<commit_message>
adding several more holes to first course, they test out fine on a device
</commit_message>
<xml_diff>
--- a/Assets/CourseDesign/Courses1.xlsx
+++ b/Assets/CourseDesign/Courses1.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17560" tabRatio="500" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="16480" yWindow="0" windowWidth="12220" windowHeight="16060" tabRatio="500" firstSheet="12" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="right-bend" sheetId="1" r:id="rId1"/>
     <sheet name="RIGHT-CORNER" sheetId="2" r:id="rId2"/>
     <sheet name="LONG-RUN" sheetId="3" r:id="rId3"/>
-    <sheet name="INCHWORM" sheetId="4" r:id="rId4"/>
+    <sheet name="Inchworm.csv" sheetId="4" r:id="rId4"/>
     <sheet name="GAMBIT" sheetId="5" r:id="rId5"/>
-    <sheet name="J" sheetId="6" r:id="rId6"/>
-    <sheet name="BONK-LINE" sheetId="7" r:id="rId7"/>
+    <sheet name="J.csv" sheetId="6" r:id="rId6"/>
+    <sheet name="Bonk-Line.csv" sheetId="7" r:id="rId7"/>
     <sheet name="MAZE" sheetId="8" r:id="rId8"/>
+    <sheet name="Mini-Jump.csv" sheetId="9" r:id="rId9"/>
+    <sheet name="Pond.csv" sheetId="10" r:id="rId10"/>
+    <sheet name="Diminish.csv" sheetId="11" r:id="rId11"/>
+    <sheet name="Curls.csv" sheetId="12" r:id="rId12"/>
+    <sheet name="Slip.csv" sheetId="13" r:id="rId13"/>
+    <sheet name="Left-Leap.csv" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="42">
   <si>
     <t>CTL</t>
   </si>
@@ -77,6 +83,81 @@
   </si>
   <si>
     <t>CBL-START</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>st</t>
+  </si>
+  <si>
+    <t>ctl</t>
+  </si>
+  <si>
+    <t>sb</t>
+  </si>
+  <si>
+    <t>sl</t>
+  </si>
+  <si>
+    <t>cbl</t>
+  </si>
+  <si>
+    <t>sr</t>
+  </si>
+  <si>
+    <t>cbr-goal</t>
+  </si>
+  <si>
+    <t>f-goal</t>
+  </si>
+  <si>
+    <t>f2</t>
+  </si>
+  <si>
+    <t>ctl-start</t>
+  </si>
+  <si>
+    <t>ctr</t>
+  </si>
+  <si>
+    <t>f2-low</t>
+  </si>
+  <si>
+    <t>f2-low-goal</t>
+  </si>
+  <si>
+    <t>ctl-low</t>
+  </si>
+  <si>
+    <t>ctr-low</t>
+  </si>
+  <si>
+    <t>sl-low</t>
+  </si>
+  <si>
+    <t>sr-low</t>
+  </si>
+  <si>
+    <t>cbr-low-goal</t>
+  </si>
+  <si>
+    <t>cbl-low</t>
+  </si>
+  <si>
+    <t>st-start</t>
+  </si>
+  <si>
+    <t>cbr</t>
+  </si>
+  <si>
+    <t>f-low</t>
+  </si>
+  <si>
+    <t>sb-low</t>
   </si>
 </sst>
 </file>
@@ -125,17 +206,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -590,6 +687,545 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="G8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="G10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="G10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
@@ -925,7 +1561,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -948,68 +1584,25 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
       <c r="C8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1017,12 +1610,6 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1220,7 +1807,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1241,51 +1828,30 @@
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="E3" t="s">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="4" spans="1:7">
       <c r="E4" t="s">
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="E5" t="s">
         <v>2</v>
       </c>
-      <c r="F5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G5" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -1294,38 +1860,20 @@
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
       <c r="C7" t="s">
         <v>3</v>
       </c>
       <c r="E7" t="s">
         <v>2</v>
-      </c>
-      <c r="F7" t="s">
-        <v>3</v>
-      </c>
-      <c r="G7" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
@@ -1334,19 +1882,10 @@
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>3</v>
-      </c>
-      <c r="G8" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
       <c r="C9" t="s">
         <v>3</v>
       </c>
@@ -1354,58 +1893,25 @@
         <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" t="s">
-        <v>3</v>
-      </c>
-      <c r="G9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
         <v>3</v>
       </c>
       <c r="F10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G10" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" t="s">
-        <v>3</v>
-      </c>
       <c r="E11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F11" t="s">
-        <v>3</v>
-      </c>
-      <c r="G11" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1421,84 +1927,227 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="D1" t="s">
+    <row r="1" spans="1:9">
+      <c r="E1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
+    <row r="2" spans="1:9">
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="F3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
       <c r="F6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="F7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="F8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="F9" t="s">
-        <v>8</v>
+        <v>19</v>
+      </c>
+      <c r="H6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" t="s">
+        <v>25</v>
+      </c>
+      <c r="I12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="I13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="I14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="I15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="I16" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1515,7 +2164,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -1691,4 +2340,69 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>